<commit_message>
add simba metadata and specific variables
</commit_message>
<xml_diff>
--- a/metadata/simba_metadata.xlsx
+++ b/metadata/simba_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA14449B-021F-364A-AE5B-FC90BBDA03EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F5A1F3-E5FF-4D43-850C-F22C6E9FAA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="500" windowWidth="25580" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16280" yWindow="500" windowWidth="20800" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>Conventions</t>
   </si>
   <si>
-    <t>CF-1.6, NCAS-AMF-1.0</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -167,12 +164,6 @@
   </si>
   <si>
     <t>v1.0</t>
-  </si>
-  <si>
-    <t>Heather Guy</t>
-  </si>
-  <si>
-    <t>heather.guy@ncas.ac.uk</t>
   </si>
   <si>
     <t>https://orcid.org/0000-0003-3525-0766</t>
@@ -262,6 +253,15 @@
   </si>
   <si>
     <t>+/- 0.0625 C</t>
+  </si>
+  <si>
+    <t>CF-1.6</t>
+  </si>
+  <si>
+    <t>heather.guy@ncas.ac.uk, michael.r.gallagher@noaa.gov</t>
+  </si>
+  <si>
+    <t>Heather Guy, Michael Gallagher</t>
   </si>
 </sst>
 </file>
@@ -731,10 +731,10 @@
   <dimension ref="A1:M1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -758,273 +758,273 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="18"/>
     </row>
     <row r="36" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="12"/>
@@ -1040,39 +1040,39 @@
     </row>
     <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" s="3"/>
     </row>
@@ -3986,7 +3986,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{FAD477BD-8341-6149-AAB9-6F510B2FFD93}"/>
+    <hyperlink ref="B10" r:id="rId1" display="heather.guy@ncas.ac.uk" xr:uid="{FAD477BD-8341-6149-AAB9-6F510B2FFD93}"/>
     <hyperlink ref="B26" r:id="rId2" xr:uid="{2B354C59-169B-5E44-B880-C90B85C249CE}"/>
     <hyperlink ref="B27" r:id="rId3" xr:uid="{2E3DC703-2B1E-0941-9307-C50FACC14B59}"/>
     <hyperlink ref="B25" r:id="rId4" xr:uid="{2969522B-5EC0-3C43-B043-B08E78BFA902}"/>

</xml_diff>